<commit_message>
Add 2017 race work
</commit_message>
<xml_diff>
--- a/ROG Budget 2017.xlsx
+++ b/ROG Budget 2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="71" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="36" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RD Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>HMRRC Race Director's Budget</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Cups</t>
-  </si>
-  <si>
-    <t>    </t>
   </si>
   <si>
     <t>Entertainment</t>
@@ -672,8 +669,8 @@
   </sheetPr>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -816,10 +813,10 @@
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="17" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
@@ -834,10 +831,10 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="17" t="n">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>3125</v>
+        <v>1925</v>
       </c>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -852,10 +849,10 @@
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="17" t="n">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>2900</v>
+        <v>1400</v>
       </c>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -869,15 +866,18 @@
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="0" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>1050</v>
+        <v>540</v>
       </c>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="I12" s="0"/>
-      <c r="J12" s="0"/>
+      <c r="J12" s="0" t="n">
+        <f aca="false">300+200+100+75+50+35+25</f>
+        <v>785</v>
+      </c>
       <c r="K12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,7 +894,9 @@
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="I13" s="0"/>
-      <c r="J13" s="0"/>
+      <c r="J13" s="0" t="n">
+        <v>261</v>
+      </c>
       <c r="K13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,7 +909,10 @@
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="I14" s="0"/>
-      <c r="J14" s="0"/>
+      <c r="J14" s="0" t="n">
+        <f aca="false">J12+J13</f>
+        <v>1046</v>
+      </c>
       <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +943,7 @@
       <c r="C16" s="22"/>
       <c r="D16" s="21" t="n">
         <f aca="false">SUM(D7:D15)</f>
-        <v>9075</v>
+        <v>5990</v>
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
@@ -1056,16 +1061,14 @@
       <c r="B25" s="15"/>
       <c r="C25" s="26"/>
       <c r="D25" s="15"/>
-      <c r="E25" s="0" t="s">
-        <v>30</v>
-      </c>
+      <c r="E25" s="0"/>
       <c r="F25" s="0"/>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="26"/>
@@ -1077,7 +1080,7 @@
     </row>
     <row r="27" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="15" t="n">
         <v>1200</v>
@@ -1087,27 +1090,27 @@
         <v>500</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F27" s="0"/>
       <c r="J27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="26"/>
       <c r="D28" s="15"/>
       <c r="E28" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="0"/>
       <c r="J28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="15" t="n">
         <v>175</v>
@@ -1117,47 +1120,47 @@
         <v>235</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="0"/>
       <c r="J29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="26"/>
       <c r="D30" s="15"/>
       <c r="E30" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F30" s="0"/>
       <c r="J30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="15" t="n">
         <v>311.5</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="28" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E31" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="26"/>
@@ -1165,13 +1168,13 @@
         <v>200</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="26"/>
@@ -1181,7 +1184,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="26"/>
@@ -1191,7 +1194,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="15" t="n">
         <v>19.44</v>
@@ -1201,13 +1204,13 @@
         <v>20</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="15" t="n">
         <v>360</v>
@@ -1217,13 +1220,13 @@
         <v>360</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="15" t="n">
         <v>243.84</v>
@@ -1233,41 +1236,41 @@
         <v>250</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="26"/>
       <c r="D38" s="15"/>
       <c r="E38" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="15" t="n">
         <v>1937.5</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="15" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="26"/>
@@ -1277,33 +1280,33 @@
     </row>
     <row r="41" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="26"/>
       <c r="D41" s="15"/>
       <c r="E41" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" s="15" t="n">
         <v>1488.3</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="15" t="n">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="E42" s="0"/>
       <c r="F42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="30"/>
@@ -1313,7 +1316,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" s="15" t="n">
         <v>122.95</v>
@@ -1323,13 +1326,13 @@
         <v>100</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F44" s="29"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="31" t="n">
         <f aca="false">SUM(B19:B44)</f>
@@ -1338,7 +1341,7 @@
       <c r="C45" s="26"/>
       <c r="D45" s="31" t="n">
         <f aca="false">SUM(D19:D44)</f>
-        <v>7465</v>
+        <v>5865</v>
       </c>
       <c r="F45" s="29"/>
     </row>
@@ -1350,7 +1353,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" s="10" t="n">
         <f aca="false">SUM(B16-B45)</f>
@@ -1359,12 +1362,12 @@
       <c r="C47" s="33"/>
       <c r="D47" s="10" t="n">
         <f aca="false">SUM(D16-D45)</f>
-        <v>1610</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" s="0"/>
       <c r="C48" s="32"/>
@@ -1372,14 +1375,14 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="34"/>
       <c r="D49" s="35"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" s="36"/>
     </row>

</xml_diff>